<commit_message>
ajustes realizados para a similaridade.
</commit_message>
<xml_diff>
--- a/detailed_interactions_cards_done_list_promos.xlsx
+++ b/detailed_interactions_cards_done_list_promos.xlsx
@@ -17445,7 +17445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17575,134 +17575,151 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>64541b8bbfe6ab6ef7939e2b</t>
+          <t>65e724b759b51ef860b3a597</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Lorenzo Villa</t>
+          <t>Julio Cesar Torres Cama</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>lorenzovilla18</t>
+          <t>julioctc</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>64d4edf4d743e8c012b275ff</t>
+          <t>64541b8bbfe6ab6ef7939e2b</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Michela Podestá</t>
+          <t>Lorenzo Villa</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>michelapodesta2</t>
+          <t>lorenzovilla18</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>64511ae29d235de041b0fc95</t>
+          <t>64d4edf4d743e8c012b275ff</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Nailea Flores</t>
+          <t>Michela Podestá</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>naileafloresd</t>
+          <t>michelapodesta2</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>649a28473d501a6d1c9e4d26</t>
+          <t>64511ae29d235de041b0fc95</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Patricia Oliva</t>
+          <t>Nailea Flores</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>poliva13</t>
+          <t>naileafloresd</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>651dad6c4df8d45af866b6e6</t>
+          <t>649a28473d501a6d1c9e4d26</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Renzo Sotelo Niquen</t>
+          <t>Patricia Oliva</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>renzosn</t>
+          <t>poliva13</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>65cc375251a5908a24b8ab6b</t>
+          <t>651dad6c4df8d45af866b6e6</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ronald Alberto Ripas Zuniga</t>
+          <t>Renzo Sotelo Niquen</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ronaldarz1</t>
+          <t>renzosn</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>63e3b73f4fcf0cb8ca0c7713</t>
+          <t>65cc375251a5908a24b8ab6b</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Valeria Mercado Mikkelsen</t>
+          <t>Ronald Alberto Ripas Zuniga</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>valeriamercadomikkelsen</t>
+          <t>ronaldarz1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>63e3b73f4fcf0cb8ca0c7713</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Valeria Mercado Mikkelsen</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>valeriamercadomikkelsen</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>65a93ddc0885439477c133de</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>joaquinaragon</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>joaquinaragon2</t>
         </is>
@@ -17918,7 +17935,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-02-26T18:33:30.613Z</t>
+          <t>2024-03-11T17:39:57.733Z</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -17967,7 +17984,7 @@
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}]</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
@@ -17984,7 +18001,7 @@
         </is>
       </c>
       <c r="W2" t="n">
-        <v>4096</v>
+        <v>212992</v>
       </c>
       <c r="X2" t="inlineStr">
         <is>
@@ -18047,7 +18064,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2024-02-26T18:33:18.701Z</t>
+          <t>2024-03-11T17:39:57.719Z</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -18103,7 +18120,7 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
@@ -18120,7 +18137,7 @@
         </is>
       </c>
       <c r="W3" t="n">
-        <v>8192</v>
+        <v>229376</v>
       </c>
       <c r="X3" t="inlineStr">
         <is>
@@ -18183,7 +18200,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2024-02-22T18:29:08.303Z</t>
+          <t>2024-03-11T17:39:57.719Z</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -18239,7 +18256,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>[{'id': '620c10bb8166f38753a39ee3', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'lime_light', 'uses': 450}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}]</t>
+          <t>[{'id': '620c10bb8166f38753a39ee3', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'lime_light', 'uses': 450}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}]</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
@@ -18256,7 +18273,7 @@
         </is>
       </c>
       <c r="W4" t="n">
-        <v>16384</v>
+        <v>245760</v>
       </c>
       <c r="X4" t="inlineStr">
         <is>
@@ -18319,7 +18336,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:42.857Z</t>
+          <t>2024-03-11T17:39:57.715Z</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -18362,7 +18379,7 @@
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -18379,7 +18396,7 @@
         </is>
       </c>
       <c r="W5" t="n">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="X5" t="inlineStr">
         <is>
@@ -18442,7 +18459,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:42.857Z</t>
+          <t>2024-03-11T17:39:57.705Z</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -18520,7 +18537,7 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>[{'id': '65aa9c7661237877872c9249', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Portal seller', 'color': 'lime', 'uses': 9}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}]</t>
+          <t>[{'id': '65aa9c7661237877872c9249', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Portal seller', 'color': 'lime', 'uses': 9}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}]</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
@@ -18537,7 +18554,7 @@
         </is>
       </c>
       <c r="W6" t="n">
-        <v>49152</v>
+        <v>278528</v>
       </c>
       <c r="X6" t="inlineStr">
         <is>
@@ -18600,7 +18617,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:42.857Z</t>
+          <t>2024-03-11T17:39:57.691Z</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -18651,7 +18668,7 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>[{'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
@@ -18668,7 +18685,7 @@
         </is>
       </c>
       <c r="W7" t="n">
-        <v>65536</v>
+        <v>294912</v>
       </c>
       <c r="X7" t="inlineStr">
         <is>
@@ -18731,7 +18748,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.776Z</t>
+          <t>2024-03-11T17:39:57.688Z</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -18800,7 +18817,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
@@ -18817,7 +18834,7 @@
         </is>
       </c>
       <c r="W8" t="n">
-        <v>81920</v>
+        <v>311296</v>
       </c>
       <c r="X8" t="inlineStr">
         <is>
@@ -18880,7 +18897,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.774Z</t>
+          <t>2024-03-11T17:39:57.688Z</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -18937,7 +18954,7 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>[{'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
@@ -18954,7 +18971,7 @@
         </is>
       </c>
       <c r="W9" t="n">
-        <v>98304</v>
+        <v>327680</v>
       </c>
       <c r="X9" t="inlineStr">
         <is>
@@ -19017,7 +19034,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.750Z</t>
+          <t>2024-03-11T17:39:57.682Z</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -19074,7 +19091,7 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
@@ -19091,7 +19108,7 @@
         </is>
       </c>
       <c r="W10" t="n">
-        <v>114688</v>
+        <v>344064</v>
       </c>
       <c r="X10" t="inlineStr">
         <is>
@@ -19154,7 +19171,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.746Z</t>
+          <t>2024-03-11T17:39:57.664Z</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -19211,7 +19228,7 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
@@ -19228,7 +19245,7 @@
         </is>
       </c>
       <c r="W11" t="n">
-        <v>131072</v>
+        <v>360448</v>
       </c>
       <c r="X11" t="inlineStr">
         <is>
@@ -19291,7 +19308,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2024-02-26T19:25:58.510Z</t>
+          <t>2024-03-11T17:39:57.661Z</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -19347,7 +19364,7 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
@@ -19364,7 +19381,7 @@
         </is>
       </c>
       <c r="W12" t="n">
-        <v>147456</v>
+        <v>376832</v>
       </c>
       <c r="X12" t="inlineStr">
         <is>
@@ -19427,7 +19444,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.742Z</t>
+          <t>2024-03-11T17:39:57.660Z</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -19491,7 +19508,7 @@
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
@@ -19508,7 +19525,7 @@
         </is>
       </c>
       <c r="W13" t="n">
-        <v>163840</v>
+        <v>393216</v>
       </c>
       <c r="X13" t="inlineStr">
         <is>
@@ -19571,7 +19588,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.715Z</t>
+          <t>2024-03-11T17:39:57.652Z</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -19628,7 +19645,7 @@
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}]</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
@@ -19645,7 +19662,7 @@
         </is>
       </c>
       <c r="W14" t="n">
-        <v>180224</v>
+        <v>409600</v>
       </c>
       <c r="X14" t="inlineStr">
         <is>
@@ -19708,7 +19725,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2024-03-01T13:09:49.056Z</t>
+          <t>2024-03-11T17:39:57.635Z</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -19768,7 +19785,7 @@
         </is>
       </c>
       <c r="W15" t="n">
-        <v>196608</v>
+        <v>425984</v>
       </c>
       <c r="X15" t="inlineStr">
         <is>
@@ -19831,7 +19848,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.711Z</t>
+          <t>2024-03-11T17:39:57.632Z</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -19895,7 +19912,7 @@
         </is>
       </c>
       <c r="W16" t="n">
-        <v>212992</v>
+        <v>442368</v>
       </c>
       <c r="X16" t="inlineStr">
         <is>
@@ -19958,7 +19975,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.704Z</t>
+          <t>2024-03-11T17:39:57.627Z</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -20022,7 +20039,7 @@
         </is>
       </c>
       <c r="W17" t="n">
-        <v>229376</v>
+        <v>458752</v>
       </c>
       <c r="X17" t="inlineStr">
         <is>
@@ -20085,7 +20102,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.688Z</t>
+          <t>2024-03-11T17:39:57.622Z</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -20137,7 +20154,7 @@
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr">
         <is>
-          <t>[{'id': '6225e2ddc5a098553aa503cd', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': '⚙️ QA', 'color': 'blue_dark', 'uses': 77}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '6225e2ddc5a098553aa503cd', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': '⚙️ QA', 'color': 'blue_dark', 'uses': 77}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
@@ -20154,7 +20171,7 @@
         </is>
       </c>
       <c r="W18" t="n">
-        <v>245760</v>
+        <v>475136</v>
       </c>
       <c r="X18" t="inlineStr">
         <is>
@@ -20217,7 +20234,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.685Z</t>
+          <t>2024-03-11T17:39:57.608Z</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -20274,7 +20291,7 @@
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
@@ -20291,7 +20308,7 @@
         </is>
       </c>
       <c r="W19" t="n">
-        <v>262144</v>
+        <v>491520</v>
       </c>
       <c r="X19" t="inlineStr">
         <is>
@@ -20354,7 +20371,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.685Z</t>
+          <t>2024-03-11T17:39:57.605Z</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -20426,7 +20443,7 @@
         </is>
       </c>
       <c r="W20" t="n">
-        <v>278528</v>
+        <v>507904</v>
       </c>
       <c r="X20" t="inlineStr">
         <is>
@@ -20489,7 +20506,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.682Z</t>
+          <t>2024-03-11T17:39:57.599Z</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -20543,7 +20560,7 @@
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
@@ -20560,7 +20577,7 @@
         </is>
       </c>
       <c r="W21" t="n">
-        <v>294912</v>
+        <v>524288</v>
       </c>
       <c r="X21" t="inlineStr">
         <is>
@@ -20623,7 +20640,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.659Z</t>
+          <t>2024-03-11T17:39:57.594Z</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -20692,7 +20709,7 @@
         </is>
       </c>
       <c r="W22" t="n">
-        <v>311296</v>
+        <v>540672</v>
       </c>
       <c r="X22" t="inlineStr">
         <is>
@@ -20755,7 +20772,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.656Z</t>
+          <t>2024-03-11T17:39:57.581Z</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -20802,7 +20819,7 @@
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
@@ -20819,7 +20836,7 @@
         </is>
       </c>
       <c r="W23" t="n">
-        <v>327680</v>
+        <v>557056</v>
       </c>
       <c r="X23" t="inlineStr">
         <is>
@@ -20882,7 +20899,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.653Z</t>
+          <t>2024-03-11T17:39:57.579Z</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -20935,7 +20952,7 @@
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
@@ -20952,7 +20969,7 @@
         </is>
       </c>
       <c r="W24" t="n">
-        <v>344064</v>
+        <v>573440</v>
       </c>
       <c r="X24" t="inlineStr">
         <is>
@@ -21015,7 +21032,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.648Z</t>
+          <t>2024-03-11T17:39:57.574Z</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -21071,7 +21088,7 @@
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
-          <t>[{'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}, {'id': '624472b10f83af06ce8db00c', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'yellow', 'uses': 12}, {'id': '620c10bb8166f38753a39ee9', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Spike 🔎', 'color': 'orange', 'uses': 25}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}, {'id': '624472b10f83af06ce8db00c', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'yellow', 'uses': 12}, {'id': '620c10bb8166f38753a39ee9', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Spike 🔎', 'color': 'orange', 'uses': 25}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
@@ -21088,7 +21105,7 @@
         </is>
       </c>
       <c r="W25" t="n">
-        <v>360448</v>
+        <v>589824</v>
       </c>
       <c r="X25" t="inlineStr">
         <is>
@@ -21155,7 +21172,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.632Z</t>
+          <t>2024-03-11T17:39:57.570Z</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
@@ -21215,7 +21232,7 @@
         </is>
       </c>
       <c r="W26" t="n">
-        <v>376832</v>
+        <v>606208</v>
       </c>
       <c r="X26" t="inlineStr">
         <is>
@@ -21278,7 +21295,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.630Z</t>
+          <t>2024-03-11T17:39:57.558Z</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -21327,7 +21344,7 @@
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}]</t>
         </is>
       </c>
       <c r="T27" t="inlineStr">
@@ -21344,7 +21361,7 @@
         </is>
       </c>
       <c r="W27" t="n">
-        <v>393216</v>
+        <v>622592</v>
       </c>
       <c r="X27" t="inlineStr">
         <is>
@@ -21407,7 +21424,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.624Z</t>
+          <t>2024-03-11T17:39:57.555Z</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -21474,7 +21491,7 @@
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr">
         <is>
-          <t>[{'id': '620c10bb8166f38753a39ee3', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'lime_light', 'uses': 450}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}]</t>
+          <t>[{'id': '620c10bb8166f38753a39ee3', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'lime_light', 'uses': 450}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}]</t>
         </is>
       </c>
       <c r="T28" t="inlineStr">
@@ -21491,7 +21508,7 @@
         </is>
       </c>
       <c r="W28" t="n">
-        <v>409600</v>
+        <v>638976</v>
       </c>
       <c r="X28" t="inlineStr">
         <is>
@@ -21554,7 +21571,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.619Z</t>
+          <t>2024-03-11T17:39:57.547Z</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -21618,7 +21635,7 @@
         </is>
       </c>
       <c r="W29" t="n">
-        <v>425984</v>
+        <v>655360</v>
       </c>
       <c r="X29" t="inlineStr">
         <is>
@@ -21681,7 +21698,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.603Z</t>
+          <t>2024-03-11T17:39:57.543Z</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -21724,7 +21741,7 @@
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T30" t="inlineStr">
@@ -21741,7 +21758,7 @@
         </is>
       </c>
       <c r="W30" t="n">
-        <v>442368</v>
+        <v>671744</v>
       </c>
       <c r="X30" t="inlineStr">
         <is>
@@ -21804,7 +21821,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.600Z</t>
+          <t>2024-03-11T17:39:57.530Z</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -21855,7 +21872,7 @@
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
         </is>
       </c>
       <c r="T31" t="inlineStr">
@@ -21872,7 +21889,7 @@
         </is>
       </c>
       <c r="W31" t="n">
-        <v>458752</v>
+        <v>688128</v>
       </c>
       <c r="X31" t="inlineStr">
         <is>
@@ -21935,7 +21952,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.589Z</t>
+          <t>2024-03-11T17:39:57.529Z</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -22004,7 +22021,7 @@
         </is>
       </c>
       <c r="W32" t="n">
-        <v>475136</v>
+        <v>704512</v>
       </c>
       <c r="X32" t="inlineStr">
         <is>
@@ -22067,7 +22084,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.584Z</t>
+          <t>2024-03-11T17:39:57.526Z</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -22127,7 +22144,7 @@
       </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
         </is>
       </c>
       <c r="T33" t="inlineStr">
@@ -22144,7 +22161,7 @@
         </is>
       </c>
       <c r="W33" t="n">
-        <v>491520</v>
+        <v>720896</v>
       </c>
       <c r="X33" t="inlineStr">
         <is>
@@ -22207,7 +22224,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.572Z</t>
+          <t>2024-03-11T17:39:57.517Z</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -22259,7 +22276,7 @@
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T34" t="inlineStr">
@@ -22276,7 +22293,7 @@
         </is>
       </c>
       <c r="W34" t="n">
-        <v>507904</v>
+        <v>737280</v>
       </c>
       <c r="X34" t="inlineStr">
         <is>
@@ -22339,7 +22356,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.572Z</t>
+          <t>2024-03-11T17:39:57.507Z</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -22382,7 +22399,7 @@
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
         </is>
       </c>
       <c r="T35" t="inlineStr">
@@ -22399,7 +22416,7 @@
         </is>
       </c>
       <c r="W35" t="n">
-        <v>524288</v>
+        <v>753664</v>
       </c>
       <c r="X35" t="inlineStr">
         <is>
@@ -22462,7 +22479,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.550Z</t>
+          <t>2024-03-11T17:39:57.505Z</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -22531,7 +22548,7 @@
         </is>
       </c>
       <c r="W36" t="n">
-        <v>540672</v>
+        <v>770048</v>
       </c>
       <c r="X36" t="inlineStr">
         <is>
@@ -22594,7 +22611,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.544Z</t>
+          <t>2024-03-11T17:39:57.500Z</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -22641,7 +22658,7 @@
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T37" t="inlineStr">
@@ -22658,7 +22675,7 @@
         </is>
       </c>
       <c r="W37" t="n">
-        <v>557056</v>
+        <v>786432</v>
       </c>
       <c r="X37" t="inlineStr">
         <is>
@@ -22721,7 +22738,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.530Z</t>
+          <t>2024-03-11T17:39:57.492Z</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -22769,7 +22786,7 @@
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>[{'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 24}]</t>
+          <t>[{'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 14}]</t>
         </is>
       </c>
       <c r="T38" t="inlineStr">
@@ -22786,7 +22803,7 @@
         </is>
       </c>
       <c r="W38" t="n">
-        <v>573440</v>
+        <v>802816</v>
       </c>
       <c r="X38" t="inlineStr">
         <is>
@@ -22849,7 +22866,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.530Z</t>
+          <t>2024-03-11T17:39:57.474Z</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -22901,7 +22918,7 @@
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>[{'id': '65143e56275ed2593c7a6059', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Android', 'color': 'green_light', 'uses': 13}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 24}]</t>
+          <t>[{'id': '65143e56275ed2593c7a6059', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Android', 'color': 'green_light', 'uses': 13}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 14}]</t>
         </is>
       </c>
       <c r="T39" t="inlineStr">
@@ -22918,7 +22935,7 @@
         </is>
       </c>
       <c r="W39" t="n">
-        <v>589824</v>
+        <v>819200</v>
       </c>
       <c r="X39" t="inlineStr">
         <is>
@@ -22981,7 +22998,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.526Z</t>
+          <t>2024-03-11T17:39:57.470Z</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -23031,7 +23048,7 @@
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 24}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 14}]</t>
         </is>
       </c>
       <c r="T40" t="inlineStr">
@@ -23048,7 +23065,7 @@
         </is>
       </c>
       <c r="W40" t="n">
-        <v>606208</v>
+        <v>835584</v>
       </c>
       <c r="X40" t="inlineStr">
         <is>
@@ -23111,7 +23128,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.514Z</t>
+          <t>2024-03-11T17:39:57.466Z</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -23170,7 +23187,7 @@
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>[{'id': '620c10bb8166f38753a39eef', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Historia de Usuario', 'color': 'blue', 'uses': 201}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 24}]</t>
+          <t>[{'id': '620c10bb8166f38753a39eef', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Historia de Usuario', 'color': 'blue', 'uses': 202}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 14}]</t>
         </is>
       </c>
       <c r="T41" t="inlineStr">
@@ -23187,7 +23204,7 @@
         </is>
       </c>
       <c r="W41" t="n">
-        <v>622592</v>
+        <v>851968</v>
       </c>
       <c r="X41" t="inlineStr">
         <is>
@@ -23250,7 +23267,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.498Z</t>
+          <t>2024-03-11T17:39:57.460Z</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -23298,7 +23315,7 @@
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 24}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 14}]</t>
         </is>
       </c>
       <c r="T42" t="inlineStr">
@@ -23315,7 +23332,7 @@
         </is>
       </c>
       <c r="W42" t="n">
-        <v>638976</v>
+        <v>868352</v>
       </c>
       <c r="X42" t="inlineStr">
         <is>
@@ -23378,7 +23395,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.495Z</t>
+          <t>2024-03-11T17:39:57.451Z</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -23425,7 +23442,7 @@
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 24}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 14}]</t>
         </is>
       </c>
       <c r="T43" t="inlineStr">
@@ -23442,7 +23459,7 @@
         </is>
       </c>
       <c r="W43" t="n">
-        <v>655360</v>
+        <v>884736</v>
       </c>
       <c r="X43" t="inlineStr">
         <is>
@@ -23505,7 +23522,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.495Z</t>
+          <t>2024-03-11T17:39:57.447Z</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -23558,7 +23575,7 @@
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 24}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 14}]</t>
         </is>
       </c>
       <c r="T44" t="inlineStr">
@@ -23575,7 +23592,7 @@
         </is>
       </c>
       <c r="W44" t="n">
-        <v>671744</v>
+        <v>901120</v>
       </c>
       <c r="X44" t="inlineStr">
         <is>
@@ -23638,7 +23655,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.489Z</t>
+          <t>2024-03-11T17:39:57.445Z</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -23681,7 +23698,7 @@
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
         </is>
       </c>
       <c r="T45" t="inlineStr">
@@ -23698,7 +23715,7 @@
         </is>
       </c>
       <c r="W45" t="n">
-        <v>688128</v>
+        <v>917504</v>
       </c>
       <c r="X45" t="inlineStr">
         <is>
@@ -23761,7 +23778,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.475Z</t>
+          <t>2024-03-11T17:39:57.437Z</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -23808,7 +23825,7 @@
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
         </is>
       </c>
       <c r="T46" t="inlineStr">
@@ -23825,7 +23842,7 @@
         </is>
       </c>
       <c r="W46" t="n">
-        <v>704512</v>
+        <v>933888</v>
       </c>
       <c r="X46" t="inlineStr">
         <is>
@@ -23888,7 +23905,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.473Z</t>
+          <t>2024-03-11T17:39:57.428Z</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -23939,7 +23956,7 @@
       </c>
       <c r="S47" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 24}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 14}]</t>
         </is>
       </c>
       <c r="T47" t="inlineStr">
@@ -23956,7 +23973,7 @@
         </is>
       </c>
       <c r="W47" t="n">
-        <v>720896</v>
+        <v>950272</v>
       </c>
       <c r="X47" t="inlineStr">
         <is>
@@ -24019,7 +24036,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.473Z</t>
+          <t>2024-03-11T17:39:57.423Z</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -24107,7 +24124,7 @@
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>[{'id': '620c10bb8166f38753a39eef', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Historia de Usuario', 'color': 'blue', 'uses': 201}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 24}]</t>
+          <t>[{'id': '620c10bb8166f38753a39eef', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Historia de Usuario', 'color': 'blue', 'uses': 202}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 14}]</t>
         </is>
       </c>
       <c r="T48" t="inlineStr">
@@ -24124,7 +24141,7 @@
         </is>
       </c>
       <c r="W48" t="n">
-        <v>737280</v>
+        <v>966656</v>
       </c>
       <c r="X48" t="inlineStr">
         <is>
@@ -24187,7 +24204,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.465Z</t>
+          <t>2024-03-11T17:39:57.415Z</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -24270,7 +24287,7 @@
         </is>
       </c>
       <c r="W49" t="n">
-        <v>753664</v>
+        <v>983040</v>
       </c>
       <c r="X49" t="inlineStr">
         <is>
@@ -24333,7 +24350,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.441Z</t>
+          <t>2024-03-11T17:39:57.402Z</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -24380,7 +24397,7 @@
       </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T50" t="inlineStr">
@@ -24397,7 +24414,7 @@
         </is>
       </c>
       <c r="W50" t="n">
-        <v>770048</v>
+        <v>999424</v>
       </c>
       <c r="X50" t="inlineStr">
         <is>
@@ -24460,7 +24477,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.436Z</t>
+          <t>2024-03-11T17:39:57.393Z</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -24513,7 +24530,7 @@
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}]</t>
         </is>
       </c>
       <c r="T51" t="inlineStr">
@@ -24530,7 +24547,7 @@
         </is>
       </c>
       <c r="W51" t="n">
-        <v>786432</v>
+        <v>1015808</v>
       </c>
       <c r="X51" t="inlineStr">
         <is>
@@ -24593,7 +24610,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.436Z</t>
+          <t>2024-03-11T17:39:57.389Z</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -24640,7 +24657,7 @@
       <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T52" t="inlineStr">
@@ -24657,7 +24674,7 @@
         </is>
       </c>
       <c r="W52" t="n">
-        <v>802816</v>
+        <v>1032192</v>
       </c>
       <c r="X52" t="inlineStr">
         <is>
@@ -24720,7 +24737,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.413Z</t>
+          <t>2024-03-11T17:39:57.377Z</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -24790,7 +24807,7 @@
         </is>
       </c>
       <c r="W53" t="n">
-        <v>819200</v>
+        <v>1048576</v>
       </c>
       <c r="X53" t="inlineStr">
         <is>
@@ -24853,7 +24870,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.413Z</t>
+          <t>2024-03-11T17:39:57.368Z</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -24917,7 +24934,7 @@
         </is>
       </c>
       <c r="W54" t="n">
-        <v>835584</v>
+        <v>1064960</v>
       </c>
       <c r="X54" t="inlineStr">
         <is>
@@ -24980,7 +24997,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.411Z</t>
+          <t>2024-03-11T17:39:57.365Z</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -25044,7 +25061,7 @@
         </is>
       </c>
       <c r="W55" t="n">
-        <v>851968</v>
+        <v>1081344</v>
       </c>
       <c r="X55" t="inlineStr">
         <is>
@@ -25107,7 +25124,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.410Z</t>
+          <t>2024-03-11T17:39:57.358Z</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -25154,7 +25171,7 @@
       <c r="R56" t="inlineStr"/>
       <c r="S56" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T56" t="inlineStr">
@@ -25171,7 +25188,7 @@
         </is>
       </c>
       <c r="W56" t="n">
-        <v>868352</v>
+        <v>1097728</v>
       </c>
       <c r="X56" t="inlineStr">
         <is>
@@ -25234,7 +25251,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2024-03-01T13:06:22.745Z</t>
+          <t>2024-03-11T17:39:57.356Z</t>
         </is>
       </c>
       <c r="G57" t="inlineStr"/>
@@ -25294,7 +25311,7 @@
         </is>
       </c>
       <c r="W57" t="n">
-        <v>884736</v>
+        <v>1114112</v>
       </c>
       <c r="X57" t="inlineStr">
         <is>
@@ -25357,7 +25374,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.391Z</t>
+          <t>2024-03-11T17:39:57.348Z</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -25425,7 +25442,7 @@
         </is>
       </c>
       <c r="W58" t="n">
-        <v>901120</v>
+        <v>1130496</v>
       </c>
       <c r="X58" t="inlineStr">
         <is>
@@ -25488,7 +25505,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.391Z</t>
+          <t>2024-03-11T17:39:57.340Z</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -25553,7 +25570,7 @@
         </is>
       </c>
       <c r="W59" t="n">
-        <v>917504</v>
+        <v>1146880</v>
       </c>
       <c r="X59" t="inlineStr">
         <is>
@@ -25616,7 +25633,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.389Z</t>
+          <t>2024-03-11T17:39:57.336Z</t>
         </is>
       </c>
       <c r="G60" t="inlineStr"/>
@@ -25659,7 +25676,7 @@
       <c r="R60" t="inlineStr"/>
       <c r="S60" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T60" t="inlineStr">
@@ -25676,7 +25693,7 @@
         </is>
       </c>
       <c r="W60" t="n">
-        <v>933888</v>
+        <v>1163264</v>
       </c>
       <c r="X60" t="inlineStr">
         <is>
@@ -25739,7 +25756,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.373Z</t>
+          <t>2024-03-11T17:39:57.333Z</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -25786,7 +25803,7 @@
       <c r="R61" t="inlineStr"/>
       <c r="S61" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T61" t="inlineStr">
@@ -25803,7 +25820,7 @@
         </is>
       </c>
       <c r="W61" t="n">
-        <v>950272</v>
+        <v>1179648</v>
       </c>
       <c r="X61" t="inlineStr">
         <is>
@@ -25866,7 +25883,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.373Z</t>
+          <t>2024-03-11T17:39:57.328Z</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -25930,7 +25947,7 @@
         </is>
       </c>
       <c r="W62" t="n">
-        <v>966656</v>
+        <v>1196032</v>
       </c>
       <c r="X62" t="inlineStr">
         <is>
@@ -25993,7 +26010,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.370Z</t>
+          <t>2024-03-11T17:39:57.320Z</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -26040,7 +26057,7 @@
       <c r="R63" t="inlineStr"/>
       <c r="S63" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T63" t="inlineStr">
@@ -26057,7 +26074,7 @@
         </is>
       </c>
       <c r="W63" t="n">
-        <v>983040</v>
+        <v>1212416</v>
       </c>
       <c r="X63" t="inlineStr">
         <is>
@@ -26120,7 +26137,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.370Z</t>
+          <t>2024-03-11T17:39:57.318Z</t>
         </is>
       </c>
       <c r="G64" t="inlineStr"/>
@@ -26163,7 +26180,7 @@
       <c r="R64" t="inlineStr"/>
       <c r="S64" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T64" t="inlineStr">
@@ -26180,7 +26197,7 @@
         </is>
       </c>
       <c r="W64" t="n">
-        <v>999424</v>
+        <v>1228800</v>
       </c>
       <c r="X64" t="inlineStr">
         <is>
@@ -26243,7 +26260,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.351Z</t>
+          <t>2024-03-11T17:39:57.313Z</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -26290,7 +26307,7 @@
       <c r="R65" t="inlineStr"/>
       <c r="S65" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T65" t="inlineStr">
@@ -26307,7 +26324,7 @@
         </is>
       </c>
       <c r="W65" t="n">
-        <v>1015808</v>
+        <v>1245184</v>
       </c>
       <c r="X65" t="inlineStr">
         <is>
@@ -26370,7 +26387,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.351Z</t>
+          <t>2024-03-11T17:39:57.307Z</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -26434,7 +26451,7 @@
         </is>
       </c>
       <c r="W66" t="n">
-        <v>1032192</v>
+        <v>1261568</v>
       </c>
       <c r="X66" t="inlineStr">
         <is>
@@ -26497,7 +26514,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.351Z</t>
+          <t>2024-03-11T17:39:57.300Z</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -26558,7 +26575,7 @@
       <c r="R67" t="inlineStr"/>
       <c r="S67" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}]</t>
         </is>
       </c>
       <c r="T67" t="inlineStr">
@@ -26575,7 +26592,7 @@
         </is>
       </c>
       <c r="W67" t="n">
-        <v>1048576</v>
+        <v>1277952</v>
       </c>
       <c r="X67" t="inlineStr">
         <is>
@@ -26638,7 +26655,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.349Z</t>
+          <t>2024-03-11T17:39:57.298Z</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -26702,7 +26719,7 @@
         </is>
       </c>
       <c r="W68" t="n">
-        <v>1064960</v>
+        <v>1294336</v>
       </c>
       <c r="X68" t="inlineStr">
         <is>
@@ -26765,7 +26782,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.332Z</t>
+          <t>2024-03-11T17:39:57.290Z</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -26821,7 +26838,7 @@
       </c>
       <c r="S69" t="inlineStr">
         <is>
-          <t>[{'id': '65143e56275ed2593c7a6059', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Android', 'color': 'green_light', 'uses': 13}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 24}]</t>
+          <t>[{'id': '65143e56275ed2593c7a6059', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Android', 'color': 'green_light', 'uses': 13}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 14}]</t>
         </is>
       </c>
       <c r="T69" t="inlineStr">
@@ -26838,7 +26855,7 @@
         </is>
       </c>
       <c r="W69" t="n">
-        <v>1081344</v>
+        <v>1310720</v>
       </c>
       <c r="X69" t="inlineStr">
         <is>
@@ -26901,7 +26918,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.332Z</t>
+          <t>2024-03-11T17:39:57.282Z</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -26950,7 +26967,7 @@
       <c r="R70" t="inlineStr"/>
       <c r="S70" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T70" t="inlineStr">
@@ -26967,7 +26984,7 @@
         </is>
       </c>
       <c r="W70" t="n">
-        <v>1097728</v>
+        <v>1327104</v>
       </c>
       <c r="X70" t="inlineStr">
         <is>
@@ -27030,7 +27047,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.332Z</t>
+          <t>2024-03-11T17:39:57.278Z</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -27081,7 +27098,7 @@
       </c>
       <c r="S71" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T71" t="inlineStr">
@@ -27098,7 +27115,7 @@
         </is>
       </c>
       <c r="W71" t="n">
-        <v>1114112</v>
+        <v>1343488</v>
       </c>
       <c r="X71" t="inlineStr">
         <is>
@@ -27161,7 +27178,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.328Z</t>
+          <t>2024-03-11T17:39:57.272Z</t>
         </is>
       </c>
       <c r="G72" t="inlineStr"/>
@@ -27204,7 +27221,7 @@
       <c r="R72" t="inlineStr"/>
       <c r="S72" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T72" t="inlineStr">
@@ -27221,7 +27238,7 @@
         </is>
       </c>
       <c r="W72" t="n">
-        <v>1130496</v>
+        <v>1359872</v>
       </c>
       <c r="X72" t="inlineStr">
         <is>
@@ -27284,7 +27301,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.310Z</t>
+          <t>2024-03-11T17:39:57.265Z</t>
         </is>
       </c>
       <c r="G73" t="inlineStr"/>
@@ -27327,7 +27344,7 @@
       <c r="R73" t="inlineStr"/>
       <c r="S73" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
         </is>
       </c>
       <c r="T73" t="inlineStr">
@@ -27344,7 +27361,7 @@
         </is>
       </c>
       <c r="W73" t="n">
-        <v>1146880</v>
+        <v>1376256</v>
       </c>
       <c r="X73" t="inlineStr">
         <is>
@@ -27407,7 +27424,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.311Z</t>
+          <t>2024-03-11T17:39:57.256Z</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -27458,7 +27475,7 @@
       </c>
       <c r="S74" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T74" t="inlineStr">
@@ -27475,7 +27492,7 @@
         </is>
       </c>
       <c r="W74" t="n">
-        <v>1163264</v>
+        <v>1392640</v>
       </c>
       <c r="X74" t="inlineStr">
         <is>
@@ -27538,7 +27555,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.309Z</t>
+          <t>2024-03-11T17:39:57.254Z</t>
         </is>
       </c>
       <c r="G75" t="inlineStr"/>
@@ -27585,7 +27602,7 @@
       </c>
       <c r="S75" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T75" t="inlineStr">
@@ -27602,7 +27619,7 @@
         </is>
       </c>
       <c r="W75" t="n">
-        <v>1179648</v>
+        <v>1409024</v>
       </c>
       <c r="X75" t="inlineStr">
         <is>
@@ -27665,7 +27682,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.309Z</t>
+          <t>2024-03-11T17:39:57.244Z</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -27717,7 +27734,7 @@
       </c>
       <c r="S76" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 24}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '64060035e007e5db60a82e75', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Siguiente Pase', 'color': 'black_dark', 'uses': 14}]</t>
         </is>
       </c>
       <c r="T76" t="inlineStr">
@@ -27734,7 +27751,7 @@
         </is>
       </c>
       <c r="W76" t="n">
-        <v>1196032</v>
+        <v>1425408</v>
       </c>
       <c r="X76" t="inlineStr">
         <is>
@@ -27797,7 +27814,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.289Z</t>
+          <t>2024-03-11T17:39:57.238Z</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -27848,7 +27865,7 @@
       </c>
       <c r="S77" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T77" t="inlineStr">
@@ -27865,7 +27882,7 @@
         </is>
       </c>
       <c r="W77" t="n">
-        <v>1212416</v>
+        <v>1441792</v>
       </c>
       <c r="X77" t="inlineStr">
         <is>
@@ -27928,7 +27945,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.289Z</t>
+          <t>2024-03-11T17:39:57.229Z</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -28009,7 +28026,7 @@
         </is>
       </c>
       <c r="W78" t="n">
-        <v>1228800</v>
+        <v>1458176</v>
       </c>
       <c r="X78" t="inlineStr">
         <is>
@@ -28072,7 +28089,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.286Z</t>
+          <t>2024-03-11T17:39:57.226Z</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -28134,7 +28151,7 @@
       <c r="R79" t="inlineStr"/>
       <c r="S79" t="inlineStr">
         <is>
-          <t>[{'id': '620c10bb8166f38753a39eef', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Historia de Usuario', 'color': 'blue', 'uses': 201}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '620c10bb8166f38753a39eef', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Historia de Usuario', 'color': 'blue', 'uses': 202}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T79" t="inlineStr">
@@ -28151,7 +28168,7 @@
         </is>
       </c>
       <c r="W79" t="n">
-        <v>1245184</v>
+        <v>1474560</v>
       </c>
       <c r="X79" t="inlineStr">
         <is>
@@ -28214,7 +28231,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.286Z</t>
+          <t>2024-03-11T17:39:57.217Z</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -28274,7 +28291,7 @@
       </c>
       <c r="S80" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T80" t="inlineStr">
@@ -28291,7 +28308,7 @@
         </is>
       </c>
       <c r="W80" t="n">
-        <v>1261568</v>
+        <v>1490944</v>
       </c>
       <c r="X80" t="inlineStr">
         <is>
@@ -28354,7 +28371,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.252Z</t>
+          <t>2024-03-11T17:39:57.214Z</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -28422,7 +28439,7 @@
         </is>
       </c>
       <c r="W81" t="n">
-        <v>1277952</v>
+        <v>1507328</v>
       </c>
       <c r="X81" t="inlineStr">
         <is>
@@ -28485,7 +28502,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.252Z</t>
+          <t>2024-03-11T17:39:57.207Z</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -28538,7 +28555,7 @@
       </c>
       <c r="S82" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T82" t="inlineStr">
@@ -28555,7 +28572,7 @@
         </is>
       </c>
       <c r="W82" t="n">
-        <v>1294336</v>
+        <v>1523712</v>
       </c>
       <c r="X82" t="inlineStr">
         <is>
@@ -28618,7 +28635,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.252Z</t>
+          <t>2024-03-11T17:39:57.205Z</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -28690,7 +28707,7 @@
       <c r="R83" t="inlineStr"/>
       <c r="S83" t="inlineStr">
         <is>
-          <t>[{'id': '620c10bb8166f38753a39eeb', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Bug', 'color': 'red', 'uses': 220}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '620c10bb8166f38753a39eeb', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Bug', 'color': 'red', 'uses': 220}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T83" t="inlineStr">
@@ -28707,7 +28724,7 @@
         </is>
       </c>
       <c r="W83" t="n">
-        <v>1310720</v>
+        <v>1540096</v>
       </c>
       <c r="X83" t="inlineStr">
         <is>
@@ -28770,7 +28787,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.250Z</t>
+          <t>2024-03-11T17:39:57.193Z</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -28821,7 +28838,7 @@
       </c>
       <c r="S84" t="inlineStr">
         <is>
-          <t>[{'id': '620c10bb8166f38753a39eeb', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Bug', 'color': 'red', 'uses': 220}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}]</t>
+          <t>[{'id': '620c10bb8166f38753a39eeb', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Bug', 'color': 'red', 'uses': 220}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}]</t>
         </is>
       </c>
       <c r="T84" t="inlineStr">
@@ -28838,7 +28855,7 @@
         </is>
       </c>
       <c r="W84" t="n">
-        <v>1327104</v>
+        <v>1556480</v>
       </c>
       <c r="X84" t="inlineStr">
         <is>
@@ -28901,7 +28918,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.194Z</t>
+          <t>2024-03-11T17:39:57.189Z</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -28948,7 +28965,7 @@
       <c r="R85" t="inlineStr"/>
       <c r="S85" t="inlineStr">
         <is>
-          <t>[{'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}, {'id': '620c10bb8166f38753a39eeb', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Bug', 'color': 'red', 'uses': 220}]</t>
+          <t>[{'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}, {'id': '620c10bb8166f38753a39eeb', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Bug', 'color': 'red', 'uses': 220}]</t>
         </is>
       </c>
       <c r="T85" t="inlineStr">
@@ -28965,7 +28982,7 @@
         </is>
       </c>
       <c r="W85" t="n">
-        <v>1343488</v>
+        <v>1572864</v>
       </c>
       <c r="X85" t="inlineStr">
         <is>
@@ -29028,7 +29045,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.193Z</t>
+          <t>2024-03-11T17:39:57.185Z</t>
         </is>
       </c>
       <c r="G86" t="inlineStr"/>
@@ -29075,7 +29092,7 @@
       </c>
       <c r="S86" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}]</t>
         </is>
       </c>
       <c r="T86" t="inlineStr">
@@ -29092,7 +29109,7 @@
         </is>
       </c>
       <c r="W86" t="n">
-        <v>1359872</v>
+        <v>1589248</v>
       </c>
       <c r="X86" t="inlineStr">
         <is>
@@ -29155,7 +29172,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.191Z</t>
+          <t>2024-03-11T17:39:57.179Z</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -29207,7 +29224,7 @@
       </c>
       <c r="S87" t="inlineStr">
         <is>
-          <t>[{'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}]</t>
+          <t>[{'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}]</t>
         </is>
       </c>
       <c r="T87" t="inlineStr">
@@ -29224,7 +29241,7 @@
         </is>
       </c>
       <c r="W87" t="n">
-        <v>1376256</v>
+        <v>1605632</v>
       </c>
       <c r="X87" t="inlineStr">
         <is>
@@ -29287,7 +29304,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2024-03-01T13:12:04.782Z</t>
+          <t>2024-03-11T17:39:57.173Z</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -29359,7 +29376,7 @@
         </is>
       </c>
       <c r="W88" t="n">
-        <v>1392640</v>
+        <v>1622016</v>
       </c>
       <c r="X88" t="inlineStr">
         <is>
@@ -29422,7 +29439,7 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.167Z</t>
+          <t>2024-03-11T17:39:57.171Z</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
@@ -29484,7 +29501,7 @@
       <c r="R89" t="inlineStr"/>
       <c r="S89" t="inlineStr">
         <is>
-          <t>[{'id': '620c10bb8166f38753a39eef', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Historia de Usuario', 'color': 'blue', 'uses': 201}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '620c10bb8166f38753a39eef', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Historia de Usuario', 'color': 'blue', 'uses': 202}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T89" t="inlineStr">
@@ -29501,7 +29518,7 @@
         </is>
       </c>
       <c r="W89" t="n">
-        <v>1409024</v>
+        <v>1638400</v>
       </c>
       <c r="X89" t="inlineStr">
         <is>
@@ -29564,7 +29581,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.163Z</t>
+          <t>2024-03-11T17:39:57.169Z</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
@@ -29617,7 +29634,7 @@
       </c>
       <c r="S90" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T90" t="inlineStr">
@@ -29634,7 +29651,7 @@
         </is>
       </c>
       <c r="W90" t="n">
-        <v>1425408</v>
+        <v>1654784</v>
       </c>
       <c r="X90" t="inlineStr">
         <is>
@@ -29697,7 +29714,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.163Z</t>
+          <t>2024-03-11T17:39:57.159Z</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -29758,7 +29775,7 @@
       <c r="R91" t="inlineStr"/>
       <c r="S91" t="inlineStr">
         <is>
-          <t>[{'id': '620c10bb8166f38753a39eef', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Historia de Usuario', 'color': 'blue', 'uses': 201}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '620c10bb8166f38753a39eef', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Historia de Usuario', 'color': 'blue', 'uses': 202}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T91" t="inlineStr">
@@ -29775,7 +29792,7 @@
         </is>
       </c>
       <c r="W91" t="n">
-        <v>1441792</v>
+        <v>1671168</v>
       </c>
       <c r="X91" t="inlineStr">
         <is>
@@ -29838,7 +29855,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.160Z</t>
+          <t>2024-03-11T17:39:57.154Z</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -29887,7 +29904,7 @@
       <c r="R92" t="inlineStr"/>
       <c r="S92" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
         </is>
       </c>
       <c r="T92" t="inlineStr">
@@ -29904,7 +29921,7 @@
         </is>
       </c>
       <c r="W92" t="n">
-        <v>1458176</v>
+        <v>1687552</v>
       </c>
       <c r="X92" t="inlineStr">
         <is>
@@ -29967,7 +29984,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.116Z</t>
+          <t>2024-03-11T17:39:57.150Z</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -30042,7 +30059,7 @@
         </is>
       </c>
       <c r="W93" t="n">
-        <v>1474560</v>
+        <v>1703936</v>
       </c>
       <c r="X93" t="inlineStr">
         <is>
@@ -30105,7 +30122,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.111Z</t>
+          <t>2024-03-11T17:39:57.149Z</t>
         </is>
       </c>
       <c r="G94" t="inlineStr"/>
@@ -30148,7 +30165,7 @@
       <c r="R94" t="inlineStr"/>
       <c r="S94" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}]</t>
         </is>
       </c>
       <c r="T94" t="inlineStr">
@@ -30165,7 +30182,7 @@
         </is>
       </c>
       <c r="W94" t="n">
-        <v>1490944</v>
+        <v>1720320</v>
       </c>
       <c r="X94" t="inlineStr">
         <is>
@@ -30228,7 +30245,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.110Z</t>
+          <t>2024-03-11T17:39:57.141Z</t>
         </is>
       </c>
       <c r="G95" t="inlineStr"/>
@@ -30271,7 +30288,7 @@
       <c r="R95" t="inlineStr"/>
       <c r="S95" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '652feb9cc7bcd78088696e5d', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BUG', 'color': 'red', 'uses': 19}]</t>
         </is>
       </c>
       <c r="T95" t="inlineStr">
@@ -30288,7 +30305,7 @@
         </is>
       </c>
       <c r="W95" t="n">
-        <v>1507328</v>
+        <v>1736704</v>
       </c>
       <c r="X95" t="inlineStr">
         <is>
@@ -30351,7 +30368,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>2024-03-01T13:10:10.103Z</t>
+          <t>2024-03-11T17:39:57.137Z</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
@@ -30398,7 +30415,7 @@
       <c r="R96" t="inlineStr"/>
       <c r="S96" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '6225e2ddc5a098553aa503cd', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': '⚙️ QA', 'color': 'blue_dark', 'uses': 77}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '6225e2ddc5a098553aa503cd', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': '⚙️ QA', 'color': 'blue_dark', 'uses': 77}]</t>
         </is>
       </c>
       <c r="T96" t="inlineStr">
@@ -30415,7 +30432,7 @@
         </is>
       </c>
       <c r="W96" t="n">
-        <v>1523712</v>
+        <v>1753088</v>
       </c>
       <c r="X96" t="inlineStr">
         <is>
@@ -30478,7 +30495,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.087Z</t>
+          <t>2024-03-11T17:39:57.135Z</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
@@ -30545,7 +30562,7 @@
       <c r="R97" t="inlineStr"/>
       <c r="S97" t="inlineStr">
         <is>
-          <t>[{'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T97" t="inlineStr">
@@ -30562,7 +30579,7 @@
         </is>
       </c>
       <c r="W97" t="n">
-        <v>1540096</v>
+        <v>1769472</v>
       </c>
       <c r="X97" t="inlineStr">
         <is>
@@ -30625,7 +30642,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.087Z</t>
+          <t>2024-03-11T17:39:57.135Z</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -30677,7 +30694,7 @@
       <c r="R98" t="inlineStr"/>
       <c r="S98" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '6285314aad97e032bb794396', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': '⚙️ Seguridad', 'color': 'sky', 'uses': 82}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '6285314aad97e032bb794396', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': '⚙️ Seguridad', 'color': 'sky', 'uses': 82}]</t>
         </is>
       </c>
       <c r="T98" t="inlineStr">
@@ -30694,7 +30711,7 @@
         </is>
       </c>
       <c r="W98" t="n">
-        <v>1556480</v>
+        <v>1785856</v>
       </c>
       <c r="X98" t="inlineStr">
         <is>
@@ -30757,7 +30774,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.082Z</t>
+          <t>2024-03-11T17:39:57.125Z</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -30804,7 +30821,7 @@
       <c r="R99" t="inlineStr"/>
       <c r="S99" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T99" t="inlineStr">
@@ -30821,7 +30838,7 @@
         </is>
       </c>
       <c r="W99" t="n">
-        <v>1572864</v>
+        <v>1802240</v>
       </c>
       <c r="X99" t="inlineStr">
         <is>
@@ -30884,7 +30901,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.078Z</t>
+          <t>2024-03-11T17:39:57.124Z</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
@@ -30931,7 +30948,7 @@
       <c r="R100" t="inlineStr"/>
       <c r="S100" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T100" t="inlineStr">
@@ -30948,7 +30965,7 @@
         </is>
       </c>
       <c r="W100" t="n">
-        <v>1589248</v>
+        <v>1818624</v>
       </c>
       <c r="X100" t="inlineStr">
         <is>
@@ -31011,7 +31028,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.058Z</t>
+          <t>2024-03-11T17:39:57.118Z</t>
         </is>
       </c>
       <c r="G101" t="inlineStr"/>
@@ -31071,7 +31088,7 @@
         </is>
       </c>
       <c r="W101" t="n">
-        <v>1605632</v>
+        <v>1835008</v>
       </c>
       <c r="X101" t="inlineStr">
         <is>
@@ -31134,7 +31151,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.059Z</t>
+          <t>2024-03-11T17:39:57.117Z</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
@@ -31183,7 +31200,7 @@
       <c r="R102" t="inlineStr"/>
       <c r="S102" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T102" t="inlineStr">
@@ -31200,7 +31217,7 @@
         </is>
       </c>
       <c r="W102" t="n">
-        <v>1622016</v>
+        <v>1851392</v>
       </c>
       <c r="X102" t="inlineStr">
         <is>
@@ -31263,7 +31280,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.057Z</t>
+          <t>2024-03-11T17:39:57.102Z</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -31316,7 +31333,7 @@
       <c r="R103" t="inlineStr"/>
       <c r="S103" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T103" t="inlineStr">
@@ -31333,7 +31350,7 @@
         </is>
       </c>
       <c r="W103" t="n">
-        <v>1638400</v>
+        <v>1867776</v>
       </c>
       <c r="X103" t="inlineStr">
         <is>
@@ -31396,7 +31413,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.055Z</t>
+          <t>2024-03-11T17:39:57.100Z</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -31460,7 +31477,7 @@
       </c>
       <c r="S104" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T104" t="inlineStr">
@@ -31477,7 +31494,7 @@
         </is>
       </c>
       <c r="W104" t="n">
-        <v>1654784</v>
+        <v>1884160</v>
       </c>
       <c r="X104" t="inlineStr">
         <is>
@@ -31540,7 +31557,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.031Z</t>
+          <t>2024-03-11T17:39:57.100Z</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
@@ -31587,7 +31604,7 @@
       <c r="R105" t="inlineStr"/>
       <c r="S105" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
         </is>
       </c>
       <c r="T105" t="inlineStr">
@@ -31604,7 +31621,7 @@
         </is>
       </c>
       <c r="W105" t="n">
-        <v>1671168</v>
+        <v>1900544</v>
       </c>
       <c r="X105" t="inlineStr">
         <is>
@@ -31667,7 +31684,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.031Z</t>
+          <t>2024-03-11T17:39:57.095Z</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -31725,7 +31742,7 @@
       <c r="R106" t="inlineStr"/>
       <c r="S106" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T106" t="inlineStr">
@@ -31742,7 +31759,7 @@
         </is>
       </c>
       <c r="W106" t="n">
-        <v>1687552</v>
+        <v>1916928</v>
       </c>
       <c r="X106" t="inlineStr">
         <is>
@@ -31805,7 +31822,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>2024-03-01T13:09:56.551Z</t>
+          <t>2024-03-11T17:39:57.075Z</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
@@ -31873,7 +31890,7 @@
         </is>
       </c>
       <c r="W107" t="n">
-        <v>1703936</v>
+        <v>1933312</v>
       </c>
       <c r="X107" t="inlineStr">
         <is>
@@ -31936,7 +31953,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.029Z</t>
+          <t>2024-03-11T17:39:57.074Z</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -31984,7 +32001,7 @@
       <c r="R108" t="inlineStr"/>
       <c r="S108" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}]</t>
         </is>
       </c>
       <c r="T108" t="inlineStr">
@@ -32001,7 +32018,7 @@
         </is>
       </c>
       <c r="W108" t="n">
-        <v>1720320</v>
+        <v>1949696</v>
       </c>
       <c r="X108" t="inlineStr">
         <is>
@@ -32064,7 +32081,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.013Z</t>
+          <t>2024-03-11T17:39:57.066Z</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -32143,7 +32160,7 @@
         </is>
       </c>
       <c r="W109" t="n">
-        <v>1736704</v>
+        <v>1966080</v>
       </c>
       <c r="X109" t="inlineStr">
         <is>
@@ -32206,7 +32223,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.013Z</t>
+          <t>2024-03-11T17:39:57.060Z</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
@@ -32254,7 +32271,7 @@
       <c r="R110" t="inlineStr"/>
       <c r="S110" t="inlineStr">
         <is>
-          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T110" t="inlineStr">
@@ -32271,7 +32288,7 @@
         </is>
       </c>
       <c r="W110" t="n">
-        <v>1753088</v>
+        <v>1982464</v>
       </c>
       <c r="X110" t="inlineStr">
         <is>
@@ -32334,7 +32351,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.013Z</t>
+          <t>2024-03-11T17:39:57.043Z</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
@@ -32383,7 +32400,7 @@
       <c r="R111" t="inlineStr"/>
       <c r="S111" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '620c10bb8166f38753a39eeb', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Bug', 'color': 'red', 'uses': 220}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '620c10bb8166f38753a39eeb', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Bug', 'color': 'red', 'uses': 220}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}]</t>
         </is>
       </c>
       <c r="T111" t="inlineStr">
@@ -32400,7 +32417,7 @@
         </is>
       </c>
       <c r="W111" t="n">
-        <v>1769472</v>
+        <v>1998848</v>
       </c>
       <c r="X111" t="inlineStr">
         <is>
@@ -32463,7 +32480,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:49.012Z</t>
+          <t>2024-03-11T17:39:57.043Z</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
@@ -32514,7 +32531,7 @@
       </c>
       <c r="S112" t="inlineStr">
         <is>
-          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 59}]</t>
+          <t>[{'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '64594c595c4896c96d51dc92', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'FE', 'color': 'purple_dark', 'uses': 69}]</t>
         </is>
       </c>
       <c r="T112" t="inlineStr">
@@ -32531,7 +32548,7 @@
         </is>
       </c>
       <c r="W112" t="n">
-        <v>1785856</v>
+        <v>2015232</v>
       </c>
       <c r="X112" t="inlineStr">
         <is>
@@ -32594,7 +32611,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.999Z</t>
+          <t>2024-03-11T17:39:57.037Z</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
@@ -32653,7 +32670,7 @@
       <c r="R113" t="inlineStr"/>
       <c r="S113" t="inlineStr">
         <is>
-          <t>[{'id': '620c10bb8166f38753a39eef', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Historia de Usuario', 'color': 'blue', 'uses': 201}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 47}]</t>
+          <t>[{'id': '620c10bb8166f38753a39eef', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Historia de Usuario', 'color': 'blue', 'uses': 202}, {'id': '65088ca05745328b712e6b74', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Campañas de canje', 'color': 'green_light', 'uses': 48}]</t>
         </is>
       </c>
       <c r="T113" t="inlineStr">
@@ -32670,7 +32687,7 @@
         </is>
       </c>
       <c r="W113" t="n">
-        <v>1802240</v>
+        <v>2031616</v>
       </c>
       <c r="X113" t="inlineStr">
         <is>
@@ -32733,7 +32750,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.996Z</t>
+          <t>2024-03-11T17:39:57.029Z</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
@@ -32788,7 +32805,7 @@
       </c>
       <c r="S114" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '6515a17446c4d8472b171314', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Stock en Linea', 'color': 'orange_dark', 'uses': 1}, {'id': '620c10bb8166f38753a39ee3', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'lime_light', 'uses': 450}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '6515a17446c4d8472b171314', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Stock en Linea', 'color': 'orange_dark', 'uses': 1}, {'id': '620c10bb8166f38753a39ee3', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'lime_light', 'uses': 450}]</t>
         </is>
       </c>
       <c r="T114" t="inlineStr">
@@ -32805,7 +32822,7 @@
         </is>
       </c>
       <c r="W114" t="n">
-        <v>1818624</v>
+        <v>2048000</v>
       </c>
       <c r="X114" t="inlineStr">
         <is>
@@ -32868,7 +32885,7 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.996Z</t>
+          <t>2024-03-11T17:39:57.008Z</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -32948,7 +32965,7 @@
         </is>
       </c>
       <c r="W115" t="n">
-        <v>1835008</v>
+        <v>2064384</v>
       </c>
       <c r="X115" t="inlineStr">
         <is>
@@ -33011,7 +33028,7 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.994Z</t>
+          <t>2024-03-11T17:39:57.007Z</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
@@ -33075,7 +33092,7 @@
         </is>
       </c>
       <c r="W116" t="n">
-        <v>1851392</v>
+        <v>2080768</v>
       </c>
       <c r="X116" t="inlineStr">
         <is>
@@ -33138,7 +33155,7 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.981Z</t>
+          <t>2024-03-11T17:39:57.005Z</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
@@ -33185,7 +33202,7 @@
       <c r="R117" t="inlineStr"/>
       <c r="S117" t="inlineStr">
         <is>
-          <t>[{'id': '624472b10f83af06ce8db00c', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'yellow', 'uses': 12}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '624472b10f83af06ce8db00c', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'yellow', 'uses': 12}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T117" t="inlineStr">
@@ -33202,7 +33219,7 @@
         </is>
       </c>
       <c r="W117" t="n">
-        <v>1867776</v>
+        <v>2097152</v>
       </c>
       <c r="X117" t="inlineStr">
         <is>
@@ -33265,7 +33282,7 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.979Z</t>
+          <t>2024-03-11T17:39:56.998Z</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
@@ -33333,7 +33350,7 @@
         </is>
       </c>
       <c r="W118" t="n">
-        <v>1884160</v>
+        <v>2113536</v>
       </c>
       <c r="X118" t="inlineStr">
         <is>
@@ -33396,7 +33413,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.979Z</t>
+          <t>2024-03-11T17:39:56.989Z</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
@@ -33468,7 +33485,7 @@
         </is>
       </c>
       <c r="W119" t="n">
-        <v>1900544</v>
+        <v>2129920</v>
       </c>
       <c r="X119" t="inlineStr">
         <is>
@@ -33531,7 +33548,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.978Z</t>
+          <t>2024-03-11T17:39:56.986Z</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
@@ -33617,7 +33634,7 @@
         </is>
       </c>
       <c r="W120" t="n">
-        <v>1916928</v>
+        <v>2146304</v>
       </c>
       <c r="X120" t="inlineStr">
         <is>
@@ -33680,7 +33697,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.964Z</t>
+          <t>2024-03-11T17:39:56.980Z</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
@@ -33748,7 +33765,7 @@
         </is>
       </c>
       <c r="W121" t="n">
-        <v>1933312</v>
+        <v>2162688</v>
       </c>
       <c r="X121" t="inlineStr">
         <is>
@@ -33811,7 +33828,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.963Z</t>
+          <t>2024-03-11T17:39:56.976Z</t>
         </is>
       </c>
       <c r="G122" t="inlineStr"/>
@@ -33871,7 +33888,7 @@
         </is>
       </c>
       <c r="W122" t="n">
-        <v>1949696</v>
+        <v>2179072</v>
       </c>
       <c r="X122" t="inlineStr">
         <is>
@@ -33934,7 +33951,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>2024-03-01T13:10:04.737Z</t>
+          <t>2024-03-11T17:39:56.965Z</t>
         </is>
       </c>
       <c r="G123" t="inlineStr"/>
@@ -33994,7 +34011,7 @@
         </is>
       </c>
       <c r="W123" t="n">
-        <v>1966080</v>
+        <v>2195456</v>
       </c>
       <c r="X123" t="inlineStr">
         <is>
@@ -34057,7 +34074,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>2024-03-01T13:10:15.663Z</t>
+          <t>2024-03-11T17:39:56.963Z</t>
         </is>
       </c>
       <c r="G124" t="inlineStr"/>
@@ -34117,7 +34134,7 @@
         </is>
       </c>
       <c r="W124" t="n">
-        <v>1982464</v>
+        <v>2211840</v>
       </c>
       <c r="X124" t="inlineStr">
         <is>
@@ -34180,7 +34197,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.945Z</t>
+          <t>2024-03-11T17:39:56.957Z</t>
         </is>
       </c>
       <c r="G125" t="inlineStr"/>
@@ -34223,7 +34240,7 @@
       <c r="R125" t="inlineStr"/>
       <c r="S125" t="inlineStr">
         <is>
-          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 38}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}]</t>
+          <t>[{'id': '620ca825880df92a80bd0a60', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'green', 'uses': 86}, {'id': '64594c4309a07cdb19a58d43', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'BE', 'color': 'orange_light', 'uses': 42}, {'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}]</t>
         </is>
       </c>
       <c r="T125" t="inlineStr">
@@ -34240,7 +34257,7 @@
         </is>
       </c>
       <c r="W125" t="n">
-        <v>1998848</v>
+        <v>2228224</v>
       </c>
       <c r="X125" t="inlineStr">
         <is>
@@ -34303,7 +34320,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.945Z</t>
+          <t>2024-03-11T17:39:56.953Z</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -34376,7 +34393,7 @@
       <c r="R126" t="inlineStr"/>
       <c r="S126" t="inlineStr">
         <is>
-          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 65}, {'id': '620c10bb8166f38753a39ee3', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'lime_light', 'uses': 450}]</t>
+          <t>[{'id': '64c02eaff71d6159d04cedaf', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'PROMOS', 'color': 'green', 'uses': 67}, {'id': '620c10bb8166f38753a39ee3', 'idBoard': '620c10ba5cfd7d4ce889d72a', 'name': 'Tarea Técnica', 'color': 'lime_light', 'uses': 450}]</t>
         </is>
       </c>
       <c r="T126" t="inlineStr">
@@ -34393,7 +34410,7 @@
         </is>
       </c>
       <c r="W126" t="n">
-        <v>2015232</v>
+        <v>2244608</v>
       </c>
       <c r="X126" t="inlineStr">
         <is>
@@ -34456,7 +34473,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.945Z</t>
+          <t>2024-03-11T17:39:56.943Z</t>
         </is>
       </c>
       <c r="G127" t="inlineStr"/>
@@ -34516,7 +34533,7 @@
         </is>
       </c>
       <c r="W127" t="n">
-        <v>2031616</v>
+        <v>2260992</v>
       </c>
       <c r="X127" t="inlineStr">
         <is>
@@ -34579,7 +34596,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.943Z</t>
+          <t>2024-03-11T17:39:56.913Z</t>
         </is>
       </c>
       <c r="G128" t="inlineStr"/>
@@ -34639,7 +34656,7 @@
         </is>
       </c>
       <c r="W128" t="n">
-        <v>2048000</v>
+        <v>2277376</v>
       </c>
       <c r="X128" t="inlineStr">
         <is>
@@ -34702,7 +34719,7 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.927Z</t>
+          <t>2024-03-11T17:39:56.909Z</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
@@ -34768,7 +34785,7 @@
         </is>
       </c>
       <c r="W129" t="n">
-        <v>2064384</v>
+        <v>2293760</v>
       </c>
       <c r="X129" t="inlineStr">
         <is>
@@ -34831,7 +34848,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>2024-02-22T18:28:48.927Z</t>
+          <t>2024-03-11T17:39:56.899Z</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
@@ -34896,7 +34913,7 @@
         </is>
       </c>
       <c r="W130" t="n">
-        <v>2080768</v>
+        <v>2310144</v>
       </c>
       <c r="X130" t="inlineStr">
         <is>

</xml_diff>